<commit_message>
[IMP] Modified: Added new books to the list
</commit_message>
<xml_diff>
--- a/Listado de Libros de lectura.xlsx
+++ b/Listado de Libros de lectura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\LocalRepo Books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{959D8D5F-1B11-4FEB-B4C4-7A66D34EA49C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46448E84-0024-4969-9DE1-58A4D6D5EA18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BEA46873-EA84-4003-9601-92B8E5BAC75C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Listado de libros de lectura</t>
   </si>
@@ -141,6 +141,30 @@
   </si>
   <si>
     <t>Phillip K. Dick</t>
+  </si>
+  <si>
+    <t>El mundo de Sofia</t>
+  </si>
+  <si>
+    <t>Jostien Gaarder</t>
+  </si>
+  <si>
+    <t>Los hermanos Karamazov</t>
+  </si>
+  <si>
+    <t>Fyodor Dostoyevsky</t>
+  </si>
+  <si>
+    <t>Thus Spoke Zarathustra</t>
+  </si>
+  <si>
+    <t>Friederich Nietzcha</t>
+  </si>
+  <si>
+    <t>El Principe</t>
+  </si>
+  <si>
+    <t>Nicolas Maquiavelo</t>
   </si>
 </sst>
 </file>
@@ -212,8 +236,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{39C2D526-702A-470D-BF9A-09A1F094C2E3}" name="Tabla1" displayName="Tabla1" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15" xr:uid="{F8E03919-48D2-4A92-9321-2F2430740995}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{39C2D526-702A-470D-BF9A-09A1F094C2E3}" name="Tabla1" displayName="Tabla1" ref="A1:C19" totalsRowShown="0">
+  <autoFilter ref="A1:C19" xr:uid="{F8E03919-48D2-4A92-9321-2F2430740995}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EC229CF0-3E70-4FB9-A9C7-D6E84D2CA72E}" name="Listado de libros de lectura"/>
     <tableColumn id="2" xr3:uid="{25F8B193-0726-4BF6-A171-168DDC7578C6}" name="Columna1"/>
@@ -520,16 +544,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DE3033-4F29-48D3-934C-3CDF2D1EE37F}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -695,6 +719,50 @@
       </c>
       <c r="C15" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>